<commit_message>
Added comments to Physics
</commit_message>
<xml_diff>
--- a/PJTagebücher_Timetracker/TimeTrackerSimon.xlsx
+++ b/PJTagebücher_Timetracker/TimeTrackerSimon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -295,7 +295,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>

</xml_diff>